<commit_message>
updated social media presence
</commit_message>
<xml_diff>
--- a/Austen/ASMR_data.xlsx
+++ b/Austen/ASMR_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JF\Documents\WASHUDATAANALYTICS\PROJECT2\YouTube-Data-Analytics-and-Visualization\Austen\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6162E112-41F7-4F8E-AFA9-DAB814E0502F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B2CDDC8-4CAB-4771-8563-138F0070440C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{A1AA5C74-36DA-4011-A64D-CAC40CC803C6}"/>
+    <workbookView xWindow="2200" yWindow="1030" windowWidth="14400" windowHeight="7360" xr2:uid="{A1AA5C74-36DA-4011-A64D-CAC40CC803C6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="82">
   <si>
     <t>Rank</t>
   </si>
@@ -265,6 +265,18 @@
   </si>
   <si>
     <t>suellASMR</t>
+  </si>
+  <si>
+    <t>twitter</t>
+  </si>
+  <si>
+    <t>instagram</t>
+  </si>
+  <si>
+    <t>twitch</t>
+  </si>
+  <si>
+    <t>facebook</t>
   </si>
 </sst>
 </file>
@@ -631,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AA450C8-68B2-4E31-AC4F-BCFC820545CD}">
-  <dimension ref="A1:L251"/>
+  <dimension ref="A1:O251"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -642,14 +654,15 @@
     <col min="1" max="1" width="9.26953125" style="4" customWidth="1"/>
     <col min="2" max="2" width="21.81640625" customWidth="1"/>
     <col min="3" max="4" width="15.54296875" customWidth="1"/>
-    <col min="5" max="5" width="17.26953125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.26953125" customWidth="1"/>
+    <col min="6" max="6" width="14.26953125" customWidth="1"/>
     <col min="7" max="7" width="15.36328125" customWidth="1"/>
     <col min="8" max="8" width="16.7265625" customWidth="1"/>
+    <col min="9" max="10" width="8.7265625" customWidth="1"/>
     <col min="11" max="11" width="12.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -683,8 +696,20 @@
       <c r="K1" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" t="s">
+        <v>79</v>
+      </c>
+      <c r="N1" t="s">
+        <v>80</v>
+      </c>
+      <c r="O1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -712,8 +737,20 @@
       <c r="K2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2">
+        <v>1</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A3" s="4">
         <v>2</v>
       </c>
@@ -748,8 +785,20 @@
       <c r="K3" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L3">
+        <v>1</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+      <c r="N3">
+        <v>1</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A4" s="4">
         <v>3</v>
       </c>
@@ -784,8 +833,20 @@
       <c r="K4" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+      <c r="N4">
+        <v>0</v>
+      </c>
+      <c r="O4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A5" s="4">
         <v>4</v>
       </c>
@@ -820,8 +881,20 @@
       <c r="K5" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L5">
+        <v>1</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
+      </c>
+      <c r="O5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A6" s="4">
         <v>5</v>
       </c>
@@ -856,8 +929,20 @@
       <c r="K6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L6">
+        <v>1</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+      <c r="N6">
+        <v>1</v>
+      </c>
+      <c r="O6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A7" s="4">
         <v>6</v>
       </c>
@@ -892,8 +977,20 @@
       <c r="K7" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L7">
+        <v>1</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>1</v>
+      </c>
+      <c r="O7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A8" s="4">
         <v>7</v>
       </c>
@@ -928,8 +1025,20 @@
       <c r="K8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L8">
+        <v>1</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+      <c r="N8">
+        <v>0</v>
+      </c>
+      <c r="O8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A9" s="4">
         <v>8</v>
       </c>
@@ -964,8 +1073,20 @@
       <c r="K9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L9">
+        <v>1</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+      <c r="N9">
+        <v>1</v>
+      </c>
+      <c r="O9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A10" s="4">
         <v>9</v>
       </c>
@@ -1000,8 +1121,20 @@
       <c r="K10" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L10">
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A11" s="4">
         <v>10</v>
       </c>
@@ -1035,8 +1168,20 @@
       <c r="K11" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L11">
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A12" s="4">
         <v>11</v>
       </c>
@@ -1064,8 +1209,20 @@
       <c r="K12" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A13" s="4">
         <v>12</v>
       </c>
@@ -1100,8 +1257,20 @@
       <c r="K13" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="N13">
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A14" s="4">
         <v>13</v>
       </c>
@@ -1136,8 +1305,20 @@
       <c r="K14" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="M14">
+        <v>0</v>
+      </c>
+      <c r="N14">
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A15" s="4">
         <v>14</v>
       </c>
@@ -1172,8 +1353,20 @@
       <c r="K15" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L15">
+        <v>1</v>
+      </c>
+      <c r="M15">
+        <v>0</v>
+      </c>
+      <c r="N15">
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A16" s="4">
         <v>15</v>
       </c>
@@ -1207,8 +1400,20 @@
       <c r="K16" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>0</v>
+      </c>
+      <c r="N16">
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A17" s="4">
         <v>16</v>
       </c>
@@ -1243,8 +1448,20 @@
       <c r="K17" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L17">
+        <v>1</v>
+      </c>
+      <c r="M17">
+        <v>1</v>
+      </c>
+      <c r="N17">
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A18" s="4">
         <v>17</v>
       </c>
@@ -1278,8 +1495,20 @@
       <c r="K18" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L18">
+        <v>1</v>
+      </c>
+      <c r="M18">
+        <v>1</v>
+      </c>
+      <c r="N18">
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A19" s="4">
         <v>18</v>
       </c>
@@ -1314,8 +1543,20 @@
       <c r="K19" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L19">
+        <v>1</v>
+      </c>
+      <c r="M19">
+        <v>1</v>
+      </c>
+      <c r="N19">
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A20" s="4">
         <v>19</v>
       </c>
@@ -1350,8 +1591,20 @@
       <c r="K20" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L20">
+        <v>0</v>
+      </c>
+      <c r="M20">
+        <v>1</v>
+      </c>
+      <c r="N20">
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A21" s="4">
         <v>20</v>
       </c>
@@ -1386,8 +1639,20 @@
       <c r="K21" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L21">
+        <v>1</v>
+      </c>
+      <c r="M21">
+        <v>0</v>
+      </c>
+      <c r="N21">
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A22" s="4">
         <v>21</v>
       </c>
@@ -1422,8 +1687,20 @@
       <c r="K22" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L22">
+        <v>1</v>
+      </c>
+      <c r="M22">
+        <v>1</v>
+      </c>
+      <c r="N22">
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A23" s="4">
         <v>22</v>
       </c>
@@ -1458,8 +1735,20 @@
       <c r="K23" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L23">
+        <v>1</v>
+      </c>
+      <c r="M23">
+        <v>0</v>
+      </c>
+      <c r="N23">
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A24" s="4">
         <v>23</v>
       </c>
@@ -1494,8 +1783,20 @@
       <c r="K24" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L24">
+        <v>0</v>
+      </c>
+      <c r="M24">
+        <v>0</v>
+      </c>
+      <c r="N24">
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A25" s="4">
         <v>24</v>
       </c>
@@ -1523,8 +1824,20 @@
       <c r="K25" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L25">
+        <v>1</v>
+      </c>
+      <c r="M25">
+        <v>0</v>
+      </c>
+      <c r="N25">
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A26" s="4">
         <v>25</v>
       </c>
@@ -1552,8 +1865,20 @@
       <c r="K26" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L26">
+        <v>0</v>
+      </c>
+      <c r="M26">
+        <v>0</v>
+      </c>
+      <c r="N26">
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A27" s="4">
         <v>26</v>
       </c>
@@ -1588,8 +1913,20 @@
       <c r="K27" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L27">
+        <v>1</v>
+      </c>
+      <c r="M27">
+        <v>1</v>
+      </c>
+      <c r="N27">
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A28" s="4">
         <v>27</v>
       </c>
@@ -1624,8 +1961,20 @@
       <c r="K28" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L28">
+        <v>0</v>
+      </c>
+      <c r="M28">
+        <v>0</v>
+      </c>
+      <c r="N28">
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A29" s="4">
         <v>28</v>
       </c>
@@ -1660,8 +2009,20 @@
       <c r="K29" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L29">
+        <v>0</v>
+      </c>
+      <c r="M29">
+        <v>1</v>
+      </c>
+      <c r="N29">
+        <v>0</v>
+      </c>
+      <c r="O29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A30" s="4">
         <v>29</v>
       </c>
@@ -1696,8 +2057,20 @@
       <c r="K30" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L30">
+        <v>0</v>
+      </c>
+      <c r="M30">
+        <v>1</v>
+      </c>
+      <c r="N30">
+        <v>0</v>
+      </c>
+      <c r="O30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A31" s="4">
         <v>30</v>
       </c>
@@ -1732,8 +2105,20 @@
       <c r="K31" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L31">
+        <v>0</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+      <c r="N31">
+        <v>0</v>
+      </c>
+      <c r="O31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A32" s="4">
         <v>31</v>
       </c>
@@ -1768,8 +2153,20 @@
       <c r="K32" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L32">
+        <v>1</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+      <c r="N32">
+        <v>1</v>
+      </c>
+      <c r="O32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A33" s="4">
         <v>32</v>
       </c>
@@ -1804,8 +2201,20 @@
       <c r="K33" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L33">
+        <v>1</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+      <c r="N33">
+        <v>0</v>
+      </c>
+      <c r="O33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A34" s="4">
         <v>33</v>
       </c>
@@ -1833,8 +2242,20 @@
       <c r="K34" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L34">
+        <v>1</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+      <c r="N34">
+        <v>0</v>
+      </c>
+      <c r="O34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A35" s="4">
         <v>34</v>
       </c>
@@ -1869,8 +2290,20 @@
       <c r="K35" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L35">
+        <v>0</v>
+      </c>
+      <c r="M35">
+        <v>0</v>
+      </c>
+      <c r="N35">
+        <v>1</v>
+      </c>
+      <c r="O35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A36" s="4">
         <v>35</v>
       </c>
@@ -1898,8 +2331,20 @@
       <c r="K36" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L36">
+        <v>0</v>
+      </c>
+      <c r="M36">
+        <v>0</v>
+      </c>
+      <c r="N36">
+        <v>0</v>
+      </c>
+      <c r="O36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A37" s="4">
         <v>36</v>
       </c>
@@ -1934,8 +2379,20 @@
       <c r="K37" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L37">
+        <v>1</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+      <c r="N37">
+        <v>0</v>
+      </c>
+      <c r="O37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A38" s="4">
         <v>37</v>
       </c>
@@ -1963,8 +2420,20 @@
       <c r="K38" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L38">
+        <v>1</v>
+      </c>
+      <c r="M38">
+        <v>0</v>
+      </c>
+      <c r="N38">
+        <v>0</v>
+      </c>
+      <c r="O38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A39" s="4">
         <v>38</v>
       </c>
@@ -1999,8 +2468,20 @@
       <c r="K39" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L39">
+        <v>1</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+      <c r="N39">
+        <v>0</v>
+      </c>
+      <c r="O39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A40" s="4">
         <v>39</v>
       </c>
@@ -2035,8 +2516,20 @@
       <c r="K40" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L40">
+        <v>1</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+      <c r="N40">
+        <v>0</v>
+      </c>
+      <c r="O40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A41" s="4">
         <v>40</v>
       </c>
@@ -2071,8 +2564,20 @@
       <c r="K41" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L41">
+        <v>1</v>
+      </c>
+      <c r="M41">
+        <v>0</v>
+      </c>
+      <c r="N41">
+        <v>0</v>
+      </c>
+      <c r="O41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A42" s="4">
         <v>41</v>
       </c>
@@ -2100,8 +2605,20 @@
       <c r="K42" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L42">
+        <v>1</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+      <c r="N42">
+        <v>0</v>
+      </c>
+      <c r="O42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A43" s="4">
         <v>42</v>
       </c>
@@ -2136,9 +2653,20 @@
       <c r="K43" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L43" s="1"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L43" s="1">
+        <v>0</v>
+      </c>
+      <c r="M43">
+        <v>0</v>
+      </c>
+      <c r="N43">
+        <v>0</v>
+      </c>
+      <c r="O43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A44" s="4">
         <v>43</v>
       </c>
@@ -2173,8 +2701,20 @@
       <c r="K44" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L44">
+        <v>1</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+      <c r="N44">
+        <v>0</v>
+      </c>
+      <c r="O44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A45" s="4">
         <v>44</v>
       </c>
@@ -2209,8 +2749,20 @@
       <c r="K45" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L45">
+        <v>1</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A46" s="4">
         <v>45</v>
       </c>
@@ -2245,8 +2797,20 @@
       <c r="K46" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>0</v>
+      </c>
+      <c r="O46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A47" s="4">
         <v>46</v>
       </c>
@@ -2274,8 +2838,20 @@
       <c r="K47" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="L47">
+        <v>1</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+      <c r="N47">
+        <v>0</v>
+      </c>
+      <c r="O47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A48" s="4">
         <v>47</v>
       </c>
@@ -2303,8 +2879,20 @@
       <c r="K48" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L48">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>0</v>
+      </c>
+      <c r="N48">
+        <v>0</v>
+      </c>
+      <c r="O48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A49" s="4">
         <v>48</v>
       </c>
@@ -2339,8 +2927,20 @@
       <c r="K49" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L49">
+        <v>1</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+      <c r="N49">
+        <v>0</v>
+      </c>
+      <c r="O49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A50" s="4">
         <v>49</v>
       </c>
@@ -2375,8 +2975,20 @@
       <c r="K50" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L50">
+        <v>1</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+      <c r="N50">
+        <v>0</v>
+      </c>
+      <c r="O50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.35">
       <c r="A51" s="4">
         <v>50</v>
       </c>
@@ -2411,56 +3023,68 @@
       <c r="K51" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.35">
+      <c r="L51">
+        <v>1</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+      <c r="N51">
+        <v>0</v>
+      </c>
+      <c r="O51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:15" x14ac:dyDescent="0.35">
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:15" x14ac:dyDescent="0.35">
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:15" x14ac:dyDescent="0.35">
       <c r="H64" s="1"/>
       <c r="I64" s="1"/>
     </row>

</xml_diff>